<commit_message>
added schematic sheet template
</commit_message>
<xml_diff>
--- a/Eagle_PCB_files/BOM.xlsx
+++ b/Eagle_PCB_files/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShaneOrmonde\Documents\GitHub\Micropeak_fork\Eagle_PCB_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F953C23-332E-4A1D-83C3-80B428B107DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709A084-2FBA-4F34-8904-4CB0827ABE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated bom with correct LED
</commit_message>
<xml_diff>
--- a/Eagle_PCB_files/BOM.xlsx
+++ b/Eagle_PCB_files/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShaneOrmonde\Documents\GitHub\Micropeak_fork\Eagle_PCB_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2709A084-2FBA-4F34-8904-4CB0827ABE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E58DDB7-0F7A-41F1-B090-B74DDD4D3E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,15 +36,9 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>LTST-C194TBKT</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>160-1837-1-ND</t>
-  </si>
-  <si>
     <t>BHX1-1025-SM</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Attiny85 MCU QFN package</t>
   </si>
   <si>
-    <t xml:space="preserve">0603 Blue communication LED </t>
-  </si>
-  <si>
     <t>MS561101BA03-50</t>
   </si>
   <si>
@@ -82,6 +73,15 @@
   </si>
   <si>
     <t>Barometric pressure sensor</t>
+  </si>
+  <si>
+    <t>LO T67K-K1L2-24-Z</t>
+  </si>
+  <si>
+    <t>475-2745-1-ND</t>
+  </si>
+  <si>
+    <t>2-PLCC Orange LED</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,77 +432,77 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added resistors and caps to BOM
</commit_message>
<xml_diff>
--- a/Eagle_PCB_files/BOM.xlsx
+++ b/Eagle_PCB_files/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShaneOrmonde\Documents\GitHub\Micropeak_fork\Eagle_PCB_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E58DDB7-0F7A-41F1-B090-B74DDD4D3E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0DB593-214D-433A-845B-C5FDCB6F11C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>MFG Part Num</t>
   </si>
@@ -82,6 +82,42 @@
   </si>
   <si>
     <t>2-PLCC Orange LED</t>
+  </si>
+  <si>
+    <t>0.1uF Capacitor</t>
+  </si>
+  <si>
+    <t>RCC0402470RFKED</t>
+  </si>
+  <si>
+    <t>541-RCC0402470RFKEDCT-ND</t>
+  </si>
+  <si>
+    <t>470R 0402 resistor</t>
+  </si>
+  <si>
+    <t>100k 0402 resistor</t>
+  </si>
+  <si>
+    <t>RCA0402100KFKEDHP</t>
+  </si>
+  <si>
+    <t>541-3242-1-ND</t>
+  </si>
+  <si>
+    <t>MCS04020C4701FE000</t>
+  </si>
+  <si>
+    <t>MCS0402-4.70K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>4.7k 0402 resistor</t>
+  </si>
+  <si>
+    <t>CL05B104KO5VPNC</t>
+  </si>
+  <si>
+    <t>1276-6844-1-ND</t>
   </si>
 </sst>
 </file>
@@ -408,16 +444,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,6 +541,62 @@
         <v>15</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>